<commit_message>
excel and app fixes
</commit_message>
<xml_diff>
--- a/estudoNN.xlsx
+++ b/estudoNN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubensantos/Documents/GitHub/CR-22-23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240DF05E-2E2E-ED4B-8ADE-C4CECB22F616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE04F30D-017A-7446-AC57-ACDEE2ADB117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Digitos_Operadores" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="189">
   <si>
     <t>Função de treino</t>
   </si>
@@ -356,6 +356,298 @@
   </si>
   <si>
     <t>Testar com dividerand = 0 no segundo parametro (validacao)</t>
+  </si>
+  <si>
+    <t>74.29</t>
+  </si>
+  <si>
+    <t>61.82</t>
+  </si>
+  <si>
+    <t>56.36</t>
+  </si>
+  <si>
+    <t>77.14</t>
+  </si>
+  <si>
+    <t>68.18</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.03
+Performance Teste Média = 0.04</t>
+  </si>
+  <si>
+    <t>53.57</t>
+  </si>
+  <si>
+    <t>43.64</t>
+  </si>
+  <si>
+    <t>Em geral obtiveram-se resultados muito semelhantes ao dataset 'train' porém o que realmente marcou diferença foi o tempo de execução dos testes, que acontece devido ao numero de imagens do dataset 'start' ser significativamente menor que o dataset 'train'.</t>
+  </si>
+  <si>
+    <t>75.14</t>
+  </si>
+  <si>
+    <t>67.27</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.04
+Performance Teste Média = 0.06</t>
+  </si>
+  <si>
+    <t>66.71</t>
+  </si>
+  <si>
+    <t>57.27</t>
+  </si>
+  <si>
+    <t>Atinge um numero de épocas muito elevado nas primeiras 4 iterações.
+Tempo de execução muito elevado nas primeiras iterações  e precisão muito baixa, nas restantes a precisão foi significativamente melhor que no dataset 'train'.
+Performance Treino Média = 0.05
+Performance Teste Média = 0.06</t>
+  </si>
+  <si>
+    <t>10.57</t>
+  </si>
+  <si>
+    <t>6.35</t>
+  </si>
+  <si>
+    <t>22.86</t>
+  </si>
+  <si>
+    <t>11.82</t>
+  </si>
+  <si>
+    <t>85.45</t>
+  </si>
+  <si>
+    <t>Resultados de teste e treino muito proximos de 100% e até por vezes a atingir esse valor em grande parte dos testes.
+Performance Treino Média = 0.03
+Performance Teste Média = 0.04</t>
+  </si>
+  <si>
+    <t>5.71</t>
+  </si>
+  <si>
+    <t>7.27</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.25
+Performance Teste Média = 0.25</t>
+  </si>
+  <si>
+    <t>22.73</t>
+  </si>
+  <si>
+    <t>10.91</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.58
+Performance Teste Média = 0.58</t>
+  </si>
+  <si>
+    <t>9.09</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.59
+Performance Teste Média = 0.58</t>
+  </si>
+  <si>
+    <t>68.86</t>
+  </si>
+  <si>
+    <t>64.35</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.05
+Performance Teste Média = 0.08</t>
+  </si>
+  <si>
+    <t>85.71</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.04
+Performance Teste Média = 0.05</t>
+  </si>
+  <si>
+    <t>82.29</t>
+  </si>
+  <si>
+    <t>67.1</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.04
+Performance Teste Média = 0.07</t>
+  </si>
+  <si>
+    <t>52.86</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.09
+Performance Teste Média = 0.11</t>
+  </si>
+  <si>
+    <t>71.71</t>
+  </si>
+  <si>
+    <t>73.57</t>
+  </si>
+  <si>
+    <t>56.19</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.04
+Performance Teste Média = 0.08</t>
+  </si>
+  <si>
+    <t>64.53</t>
+  </si>
+  <si>
+    <t>61.38</t>
+  </si>
+  <si>
+    <t>77.62</t>
+  </si>
+  <si>
+    <t>40.71</t>
+  </si>
+  <si>
+    <t>83.10</t>
+  </si>
+  <si>
+    <t>68.33</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.03
+Performance Teste Média = 0.06</t>
+  </si>
+  <si>
+    <t>48.1</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.05
+Performance Teste Média = 0.07</t>
+  </si>
+  <si>
+    <t>83.1</t>
+  </si>
+  <si>
+    <t>81.67</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.02
+Performance Teste Média = 0.02</t>
+  </si>
+  <si>
+    <t>42.14</t>
+  </si>
+  <si>
+    <t>38.33</t>
+  </si>
+  <si>
+    <t>Atinge um numero de épocas muito elevado nas primeiras 4 iterações.
+Tempo de execução muito elevado nas primeiras iterações  e precisão muito baixa, nas restantes a precisão foi significativamente melhor que no dataset 'train'.
+Performance Treino Média = 0.07
+Performance Teste Média = 0.09</t>
+  </si>
+  <si>
+    <t>39.52</t>
+  </si>
+  <si>
+    <t>33.33</t>
+  </si>
+  <si>
+    <t>59.52</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.07
+Performance Teste Média = 0.08</t>
+  </si>
+  <si>
+    <t>52.14</t>
+  </si>
+  <si>
+    <t>43.33</t>
+  </si>
+  <si>
+    <t>87.62</t>
+  </si>
+  <si>
+    <t>86.67</t>
+  </si>
+  <si>
+    <t>Resultados de teste e treino muito proximos de 100% e até por vezes a atingir esse valor em grande parte dos testes.
+Performance Treino Média = 0.02
+Performance Teste Média = 0.03</t>
+  </si>
+  <si>
+    <t>30.71</t>
+  </si>
+  <si>
+    <t>18.33</t>
+  </si>
+  <si>
+    <t>8.33</t>
+  </si>
+  <si>
+    <t>4.76</t>
+  </si>
+  <si>
+    <t>3.33</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.55
+Performance Teste Média = 0.57</t>
+  </si>
+  <si>
+    <t>9.52</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.63
+Performance Teste Média = 0.62</t>
+  </si>
+  <si>
+    <t>54.29</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.08
+Performance Teste Média = 0.1</t>
+  </si>
+  <si>
+    <t>89.05</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.03
+Performance Teste Média = 0.05</t>
+  </si>
+  <si>
+    <t>62.14</t>
+  </si>
+  <si>
+    <t>62.73</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.08
+Performance Teste Média = 0.11</t>
+  </si>
+  <si>
+    <t>67.5</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.06
+Performance Teste Média = 0.09</t>
+  </si>
+  <si>
+    <t>70.24</t>
+  </si>
+  <si>
+    <t>57.69</t>
+  </si>
+  <si>
+    <t>Performance Treino Média = 0.04
+Performance Teste Média = 0.11</t>
   </si>
 </sst>
 </file>
@@ -399,6 +691,7 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -414,6 +707,7 @@
       <sz val="18"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -682,7 +976,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -711,33 +1005,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -767,8 +1039,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="73">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
@@ -1180,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1198,35 +1559,45 @@
     <col min="12" max="12" width="10.1640625" customWidth="1"/>
     <col min="13" max="13" width="20.5" customWidth="1"/>
     <col min="14" max="14" width="24.5" customWidth="1"/>
-    <col min="16" max="16" width="24.5" customWidth="1"/>
-    <col min="17" max="17" width="24.6640625" customWidth="1"/>
+    <col min="15" max="15" width="8.5" style="41" customWidth="1"/>
+    <col min="16" max="16" width="68" style="41" customWidth="1"/>
+    <col min="18" max="18" width="24.5" customWidth="1"/>
+    <col min="19" max="19" width="24.6640625" customWidth="1"/>
+    <col min="21" max="21" width="65.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:21" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="K1" s="29" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="K1" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="P1" s="20" t="s">
+      <c r="N1" s="27"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="Q1" s="21"/>
-    </row>
-    <row r="2" spans="1:17" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S1" s="27"/>
+      <c r="U1" s="44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="85" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1249,28 +1620,38 @@
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="M2" s="22" t="s">
+      <c r="K2" s="20"/>
+      <c r="M2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="O2" s="38"/>
+      <c r="P2" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="R2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="23" t="s">
+      <c r="S2" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K3" s="31"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="25"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="25"/>
-    </row>
-    <row r="4" spans="1:17" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U2" s="46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="21"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="42"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="15"/>
+      <c r="U3" s="42"/>
+    </row>
+    <row r="4" spans="1:21" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -1290,60 +1671,84 @@
         <v>11</v>
       </c>
       <c r="G4" s="7"/>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="17"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="17"/>
-    </row>
-    <row r="5" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K5" s="31"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="25"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="25"/>
-    </row>
-    <row r="6" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K6" s="31"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="25"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="25"/>
-    </row>
-    <row r="7" spans="1:17" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="M4" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" s="40"/>
+      <c r="P4" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="R4" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="S4" s="32">
+        <v>70</v>
+      </c>
+      <c r="U4" s="52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K5" s="21"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="43"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="34"/>
+      <c r="U5" s="43"/>
+    </row>
+    <row r="6" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="21"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="43"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="34"/>
+      <c r="U6" s="43"/>
+    </row>
+    <row r="7" spans="1:21" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-      <c r="K7" s="31"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="25"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="25"/>
-    </row>
-    <row r="8" spans="1:17" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
+      <c r="K7" s="21"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="43"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="34"/>
+      <c r="U7" s="43"/>
+    </row>
+    <row r="8" spans="1:21" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="17">
         <v>2</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="17" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1356,28 +1761,43 @@
         <v>11</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="K8" s="32" t="s">
+      <c r="K8" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="16"/>
-      <c r="N8" s="17"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="17"/>
-    </row>
-    <row r="9" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="M8" s="31">
+        <v>60</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="O8" s="40"/>
+      <c r="P8" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="R8" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="S8" s="32">
+        <v>35</v>
+      </c>
+      <c r="U8" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="17">
         <v>2</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -1390,28 +1810,43 @@
         <v>11</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="17"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="17"/>
-    </row>
-    <row r="10" spans="1:17" ht="103" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="M9" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="O9" s="40"/>
+      <c r="P9" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="R9" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="S9" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="U9" s="51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="18">
         <v>3</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="18" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -1424,28 +1859,43 @@
         <v>11</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="K10" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="M10" s="16"/>
-      <c r="N10" s="17"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="17"/>
-    </row>
-    <row r="11" spans="1:17" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="M10" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="N10" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" s="40"/>
+      <c r="P10" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="R10" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="S10" s="32">
+        <v>40</v>
+      </c>
+      <c r="U10" s="51" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="18">
         <v>3</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="18" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -1458,49 +1908,70 @@
         <v>11</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="32" t="s">
+      <c r="K11" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="18"/>
-      <c r="N11" s="19"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="19"/>
-    </row>
-    <row r="12" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K12" s="31"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="25"/>
-    </row>
-    <row r="13" spans="1:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="M11" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="N11" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="O11" s="40"/>
+      <c r="P11" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="R11" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="S11" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="U11" s="47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="21"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="43"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="34"/>
+      <c r="U12" s="43"/>
+    </row>
+    <row r="13" spans="1:21" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
-      <c r="K13" s="35" t="s">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+      <c r="K13" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="M13" s="24"/>
-      <c r="N13" s="25"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="25"/>
-    </row>
-    <row r="14" spans="1:17" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="M13" s="33"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="50"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="34"/>
+      <c r="U13" s="50"/>
+    </row>
+    <row r="14" spans="1:21" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="7">
@@ -1512,29 +1983,44 @@
       <c r="D14" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="17" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="13" t="s">
+      <c r="H14" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K14" s="33" t="s">
+      <c r="K14" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="M14" s="16"/>
-      <c r="N14" s="17"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="17"/>
-    </row>
-    <row r="15" spans="1:17" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="M14" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="O14" s="40"/>
+      <c r="P14" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="R14" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="S14" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="U14" s="49" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="7">
@@ -1546,29 +2032,44 @@
       <c r="D15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="17" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="K15" s="33" t="s">
+      <c r="K15" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="M15" s="16"/>
-      <c r="N15" s="17"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="17"/>
-    </row>
-    <row r="16" spans="1:17" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="M15" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="N15" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="O15" s="40"/>
+      <c r="P15" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="R15" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="S15" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="U15" s="49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="7">
@@ -1580,29 +2081,44 @@
       <c r="D16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="18" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="33" t="s">
+      <c r="K16" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="N16" s="17"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="17"/>
-    </row>
-    <row r="17" spans="1:17" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="M16" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="N16" s="32">
+        <v>30</v>
+      </c>
+      <c r="O16" s="40"/>
+      <c r="P16" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="R16" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="S16" s="32">
+        <v>45</v>
+      </c>
+      <c r="U16" s="49" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="7">
@@ -1614,60 +2130,84 @@
       <c r="D17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="18" t="s">
         <v>30</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="K17" s="33" t="s">
+      <c r="K17" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="M17" s="16"/>
-      <c r="N17" s="17"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="17"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K18" s="31"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="25"/>
-    </row>
-    <row r="19" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K19" s="31"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="25"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="25"/>
-    </row>
-    <row r="20" spans="1:17" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="M17" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="N17" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="O17" s="40"/>
+      <c r="P17" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="R17" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="S17" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="U17" s="49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="K18" s="21"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="43"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="34"/>
+      <c r="U18" s="43"/>
+    </row>
+    <row r="19" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="21"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="43"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="34"/>
+      <c r="U19" s="43"/>
+    </row>
+    <row r="20" spans="1:21" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
-      <c r="K20" s="31"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="25"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="25"/>
-    </row>
-    <row r="21" spans="1:17" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="30"/>
+      <c r="K20" s="21"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="50"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="34"/>
+      <c r="U20" s="50"/>
+    </row>
+    <row r="21" spans="1:21" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -1693,15 +2233,30 @@
       <c r="I21" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="33" t="s">
+      <c r="K21" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="M21" s="16"/>
-      <c r="N21" s="17"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="17"/>
-    </row>
-    <row r="22" spans="1:17" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M21" s="31">
+        <v>90</v>
+      </c>
+      <c r="N21" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="O21" s="40"/>
+      <c r="P21" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="R21" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="S21" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="U21" s="48" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1727,15 +2282,30 @@
       <c r="I22" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="33" t="s">
+      <c r="K22" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="M22" s="16"/>
-      <c r="N22" s="17"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="17"/>
-    </row>
-    <row r="23" spans="1:17" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M22" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="N22" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="O22" s="40"/>
+      <c r="P22" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="R22" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="S22" s="32">
+        <v>25</v>
+      </c>
+      <c r="U22" s="49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>15</v>
       </c>
@@ -1761,15 +2331,30 @@
       <c r="I23" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K23" s="33" t="s">
+      <c r="K23" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="M23" s="16"/>
-      <c r="N23" s="17"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="17"/>
-    </row>
-    <row r="24" spans="1:17" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M23" s="31">
+        <v>23</v>
+      </c>
+      <c r="N23" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="O23" s="40"/>
+      <c r="P23" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="R23" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="S23" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="U23" s="49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -1795,15 +2380,30 @@
       <c r="I24" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="K24" s="33" t="s">
+      <c r="K24" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="M24" s="16"/>
-      <c r="N24" s="17"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="17"/>
-    </row>
-    <row r="25" spans="1:17" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M24" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="N24" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="O24" s="40"/>
+      <c r="P24" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="R24" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="S24" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="U24" s="49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -1829,15 +2429,30 @@
       <c r="I25" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="K25" s="33" t="s">
+      <c r="K25" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="M25" s="16"/>
-      <c r="N25" s="17"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="17"/>
-    </row>
-    <row r="26" spans="1:17" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M25" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="N25" s="32">
+        <v>10</v>
+      </c>
+      <c r="O25" s="40"/>
+      <c r="P25" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="R25" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="S25" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="U25" s="49" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -1863,42 +2478,63 @@
       <c r="I26" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="K26" s="33" t="s">
+      <c r="K26" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="M26" s="16"/>
-      <c r="N26" s="17"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="17"/>
-    </row>
-    <row r="27" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K27" s="31"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="25"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="25"/>
-    </row>
-    <row r="28" spans="1:17" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="M26" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="N26" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="O26" s="40"/>
+      <c r="P26" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="R26" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="S26" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="U26" s="49" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="21"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="40"/>
+      <c r="P27" s="45"/>
+      <c r="R27" s="33"/>
+      <c r="S27" s="34"/>
+      <c r="U27" s="45"/>
+    </row>
+    <row r="28" spans="1:21" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="12"/>
-      <c r="K28" s="33" t="s">
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="30"/>
+      <c r="K28" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="M28" s="24"/>
-      <c r="N28" s="25"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="25"/>
-    </row>
-    <row r="29" spans="1:17" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M28" s="33"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="45"/>
+      <c r="R28" s="33"/>
+      <c r="S28" s="34"/>
+      <c r="U28" s="45"/>
+    </row>
+    <row r="29" spans="1:21" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -1924,15 +2560,30 @@
       <c r="I29" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K29" s="33" t="s">
+      <c r="K29" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="17"/>
-    </row>
-    <row r="30" spans="1:17" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M29" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="N29" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="O29" s="40"/>
+      <c r="P29" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="R29" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="S29" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="U29" s="49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>14</v>
       </c>
@@ -1958,15 +2609,30 @@
       <c r="I30" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="K30" s="33" t="s">
+      <c r="K30" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="M30" s="16"/>
-      <c r="N30" s="17"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="17"/>
-    </row>
-    <row r="31" spans="1:17" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M30" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="N30" s="32">
+        <v>80</v>
+      </c>
+      <c r="O30" s="40"/>
+      <c r="P30" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="R30" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="S30" s="32">
+        <v>75</v>
+      </c>
+      <c r="U30" s="49" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
@@ -1992,15 +2658,30 @@
       <c r="I31" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="K31" s="33" t="s">
+      <c r="K31" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="M31" s="16"/>
-      <c r="N31" s="17"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="17"/>
-    </row>
-    <row r="32" spans="1:17" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M31" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="N31" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="O31" s="40"/>
+      <c r="P31" s="49" t="s">
+        <v>138</v>
+      </c>
+      <c r="R31" s="31">
+        <v>85</v>
+      </c>
+      <c r="S31" s="32">
+        <v>75</v>
+      </c>
+      <c r="U31" s="49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
@@ -2026,15 +2707,30 @@
       <c r="I32" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="K32" s="33" t="s">
+      <c r="K32" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="M32" s="16"/>
-      <c r="N32" s="17"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="17"/>
-    </row>
-    <row r="33" spans="1:17" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M32" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="N32" s="32">
+        <v>45</v>
+      </c>
+      <c r="O32" s="40"/>
+      <c r="P32" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="R32" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="S32" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="U32" s="49" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>25</v>
       </c>
@@ -2060,15 +2756,30 @@
       <c r="I33" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="K33" s="33" t="s">
+      <c r="K33" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="M33" s="16"/>
-      <c r="N33" s="17"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="17"/>
-    </row>
-    <row r="34" spans="1:17" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M33" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="N33" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="O33" s="40"/>
+      <c r="P33" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="R33" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="S33" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="U33" s="49" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>26</v>
       </c>
@@ -2088,23 +2799,44 @@
         <v>41</v>
       </c>
       <c r="G34" s="3"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="5"/>
-      <c r="K34" s="34"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="17"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="17"/>
+      <c r="H34" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="K34" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="M34" s="31">
+        <v>64</v>
+      </c>
+      <c r="N34" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="O34" s="40"/>
+      <c r="P34" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="R34" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="S34" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="U34" s="53" t="s">
+        <v>188</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A28:I28"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
     <mergeCell ref="A7:I7"/>
     <mergeCell ref="A13:I13"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A28:I28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>